<commit_message>
Début du code du chauffage
Ajout du stockage des température
</commit_message>
<xml_diff>
--- a/Documentation/Memory_map.xlsx
+++ b/Documentation/Memory_map.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C_He_arc_1ere\projet p1\GitHub\Project_P1.X\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damien.gygi\Documents\GitHub\Project_P1.X\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Memory Map </t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>0x000E - 0x0010</t>
+  </si>
+  <si>
+    <t>Begin_temperature</t>
+  </si>
+  <si>
+    <t>0x0011- 0x0013</t>
+  </si>
+  <si>
+    <t>0x0014 - 0x0016</t>
+  </si>
+  <si>
+    <t>0x0017 - 0x0019</t>
+  </si>
+  <si>
+    <t>Actual_temperature</t>
+  </si>
+  <si>
+    <t>End_temperature</t>
   </si>
 </sst>
 </file>
@@ -145,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -153,6 +171,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -439,139 +460,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:G18"/>
+  <dimension ref="C2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="7"/>
       <c r="G4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="6" t="s">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="7"/>
       <c r="G5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="5" t="s">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="6"/>
       <c r="G6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="5" t="s">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="6"/>
       <c r="G7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="5" t="s">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="6"/>
       <c r="G8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="5" t="s">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="6"/>
       <c r="G9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E10" s="3"/>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="6" t="s">
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E17" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" t="s">
+      <c r="F17" s="7"/>
+      <c r="G17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" t="s">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E14" s="5" t="s">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" t="s">
+      <c r="F20" s="6"/>
+      <c r="G20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="5" t="s">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" t="s">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E11:F12"/>
     <mergeCell ref="E17:F18"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modification des fonctions de logins
</commit_message>
<xml_diff>
--- a/Documentation/Memory_map.xlsx
+++ b/Documentation/Memory_map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\C_He_arc_1ere\projet p1\GitHub\Project_P1.X\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohammed.bensalah\Documents\GitHub\Project_P1.X\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Memory Map </t>
   </si>
@@ -71,9 +71,6 @@
     <t>0x36D - 0x371</t>
   </si>
   <si>
-    <t>Mesure de Température</t>
-  </si>
-  <si>
     <t>Begin_post_it</t>
   </si>
   <si>
@@ -84,6 +81,27 @@
   </si>
   <si>
     <t>0x000E - 0x0010</t>
+  </si>
+  <si>
+    <t>Notes sauvegardées</t>
+  </si>
+  <si>
+    <t>0x1FFFF</t>
+  </si>
+  <si>
+    <t>0x372</t>
+  </si>
+  <si>
+    <t>Date de la sauvegarde</t>
+  </si>
+  <si>
+    <t>0x373</t>
+  </si>
+  <si>
+    <t>56 mesures de températures</t>
+  </si>
+  <si>
+    <t>0x3AB</t>
   </si>
 </sst>
 </file>
@@ -439,13 +457,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:G18"/>
+  <dimension ref="C2:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="E14" sqref="E14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -494,20 +516,20 @@
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E8" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
@@ -541,37 +563,58 @@
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E15" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F15" s="5"/>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="F16" s="5"/>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E11:F12"/>
-    <mergeCell ref="E17:F18"/>
+    <mergeCell ref="E18:F19"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mise à jour du Memory Map
</commit_message>
<xml_diff>
--- a/Documentation/Memory_map.xlsx
+++ b/Documentation/Memory_map.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damien.gygi\Documents\GitHub\Project_P1.X\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohammed.bensalah\Documents\GitHub\Project_P1.X\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">Memory Map </t>
   </si>
@@ -116,7 +116,28 @@
     <t>0x001B - 0x001D</t>
   </si>
   <si>
-    <t>0x400</t>
+    <t>0x1FFFF</t>
+  </si>
+  <si>
+    <t>Notes sauvegardées</t>
+  </si>
+  <si>
+    <t>0x400 -0x402</t>
+  </si>
+  <si>
+    <t>Date mesure de température</t>
+  </si>
+  <si>
+    <t>Heure Mesure</t>
+  </si>
+  <si>
+    <t>0x403-0x405</t>
+  </si>
+  <si>
+    <t>0x406</t>
+  </si>
+  <si>
+    <t>0x4E6</t>
   </si>
 </sst>
 </file>
@@ -178,14 +199,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -472,187 +490,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:G26"/>
+  <dimension ref="C2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="5"/>
       <c r="G4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E5" s="6" t="s">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="5"/>
       <c r="G5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E6" s="5" t="s">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="4"/>
       <c r="G6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E7" s="5" t="s">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="4"/>
       <c r="G7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="5" t="s">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="4"/>
       <c r="G8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E9" s="6" t="s">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="5"/>
       <c r="G9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E10" s="5" t="s">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="4"/>
       <c r="G10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="6" t="s">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="5"/>
       <c r="G11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="5" t="s">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="4"/>
       <c r="G12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="5" t="s">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="4"/>
       <c r="G13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="5" t="s">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="4"/>
       <c r="G14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E19" s="6" t="s">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="6"/>
+      <c r="F19" s="5"/>
       <c r="G19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="5" t="s">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="4"/>
       <c r="G22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E24" s="5"/>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="F24" s="5"/>
       <c r="G24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E25" s="4"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
+      <c r="G26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="E27:F28"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E19:F20"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F24"/>
+    <mergeCell ref="E25:F26"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E19:F20"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>